<commit_message>
adding some more testscripts
</commit_message>
<xml_diff>
--- a/src/main/java/qa/keyword/scenarios/amazon-keyword.xlsx
+++ b/src/main/java/qa/keyword/scenarios/amazon-keyword.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="signup" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -16,10 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
-  <si>
-    <t>locator</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="33">
   <si>
     <t>teststep</t>
   </si>
@@ -48,36 +45,18 @@
     <t>enter email address</t>
   </si>
   <si>
-    <t>id=username</t>
-  </si>
-  <si>
     <t>sendkeys</t>
   </si>
   <si>
     <t>enter password</t>
   </si>
   <si>
-    <t>id=password</t>
-  </si>
-  <si>
     <t>click login button</t>
   </si>
   <si>
     <t>click</t>
   </si>
   <si>
-    <t>id=loginBtn</t>
-  </si>
-  <si>
-    <t>https://app.hubspot.com/login</t>
-  </si>
-  <si>
-    <t>niranjangutha@gmail.com</t>
-  </si>
-  <si>
-    <t>niranjan@123</t>
-  </si>
-  <si>
     <t>close the browser</t>
   </si>
   <si>
@@ -87,14 +66,62 @@
     <t xml:space="preserve">click signup </t>
   </si>
   <si>
-    <t>LinkText=Sign up</t>
+    <t>locator name</t>
+  </si>
+  <si>
+    <t>locator value</t>
+  </si>
+  <si>
+    <t>LinkText</t>
+  </si>
+  <si>
+    <t>xpath</t>
+  </si>
+  <si>
+    <t>//input[@id='pass']</t>
+  </si>
+  <si>
+    <t>//input[@id='u_0_2']</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com</t>
+  </si>
+  <si>
+    <t>Forgotten account?</t>
+  </si>
+  <si>
+    <t>niranjan gutha</t>
+  </si>
+  <si>
+    <t>firefox</t>
+  </si>
+  <si>
+    <t>isDisplaed</t>
+  </si>
+  <si>
+    <t>check signup</t>
+  </si>
+  <si>
+    <t>Get url</t>
+  </si>
+  <si>
+    <t>geturl</t>
+  </si>
+  <si>
+    <t>partialLinkText</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>email</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,6 +133,11 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -134,9 +166,10 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -432,179 +465,148 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:D11"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
       <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="E3" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+      <c r="E4" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="1">
+        <v>19032014</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
         <v>13</v>
       </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
         <v>14</v>
       </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" t="s">
-        <v>5</v>
-      </c>
+      <c r="E7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="E9" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1"/>
-    <hyperlink ref="D4" r:id="rId2"/>
-    <hyperlink ref="D5" r:id="rId3"/>
-    <hyperlink ref="D9" r:id="rId4"/>
+    <hyperlink ref="E4" r:id="rId1" display="niranjangutha@gmail.com"/>
+    <hyperlink ref="E5" r:id="rId2" display="niranjan@123"/>
+    <hyperlink ref="E3" r:id="rId3" display="https://www.facebook.com/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -612,13 +614,146 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E3" r:id="rId1" display="https://www.facebook.com/"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>